<commit_message>
Chagne Detect Collision System
</commit_message>
<xml_diff>
--- a/Tools/Tables/BuildModelTable.xlsx
+++ b/Tools/Tables/BuildModelTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BuildingSystem\Tools\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A9D98E-CF76-40DD-8FA1-03940260596B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE8DAB7-8C8B-4BAA-8386-4C63CB9ACBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7755" yWindow="3015" windowWidth="29400" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,25 +221,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>가데이터1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Script/Engine.StaticMesh'/Game/LevelPrototyping/Meshes/SM_Ramp.SM_Ramp'</t>
-  </si>
-  <si>
-    <t>가데이터2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가데이터3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가데이터4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프리뷰 이미지 경로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -286,8 +267,28 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Enum 타입 0 = 바닥, 1 = 벽, 2 = 계단</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <t>Enum 타입 0 = 바닥, 1 = 벽, 2 = 계단, 3 = 지붕</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌 바닥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌 벽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무 계단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌 지붕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Script/Engine.Blueprint'/Game/BuildingSystem/Blueprints/Placeable/BP_StoneRoof.BP_StoneRoof_C'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -500,6 +501,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -516,15 +526,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,13 +1007,13 @@
     </row>
     <row r="9" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1032,9 +1033,9 @@
     </row>
     <row r="10" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1054,9 +1055,9 @@
     </row>
     <row r="11" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1076,13 +1077,13 @@
     </row>
     <row r="12" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1102,9 +1103,9 @@
     </row>
     <row r="13" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1124,9 +1125,9 @@
     </row>
     <row r="14" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1248,13 +1249,13 @@
     </row>
     <row r="20" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="14"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="5" t="s">
         <v>14</v>
       </c>
@@ -1272,9 +1273,9 @@
     </row>
     <row r="21" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="5" t="s">
         <v>29</v>
       </c>
@@ -1292,9 +1293,9 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="5" t="s">
         <v>30</v>
       </c>
@@ -1334,13 +1335,13 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="14"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="5" t="s">
         <v>14</v>
       </c>
@@ -1358,9 +1359,9 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="5" t="s">
         <v>33</v>
       </c>
@@ -1378,9 +1379,9 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="5" t="s">
         <v>34</v>
       </c>
@@ -1420,13 +1421,13 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="14"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1444,9 +1445,9 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="15"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="5" t="s">
         <v>38</v>
       </c>
@@ -1464,9 +1465,9 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="15"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="5" t="s">
         <v>39</v>
       </c>
@@ -1484,9 +1485,9 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="15"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="5" t="s">
         <v>40</v>
       </c>
@@ -1504,9 +1505,9 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="16"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="5" t="s">
         <v>41</v>
       </c>
@@ -3900,6 +3901,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="C28:C32"/>
     <mergeCell ref="D28:D32"/>
@@ -3909,12 +3916,6 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="D24:D26"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3926,8 +3927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81AEE15-75BD-4427-A913-E1C9FC07829A}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3981,16 +3982,16 @@
         <v>45</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -4001,16 +4002,16 @@
         <v>43</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4018,13 +4019,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E5" s="10">
         <v>0</v>
@@ -4038,13 +4039,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -4058,13 +4059,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E7" s="10">
         <v>2</v>
@@ -4078,16 +4079,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E8" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="10">
         <v>0</v>

</xml_diff>